<commit_message>
Zip and other changes
</commit_message>
<xml_diff>
--- a/Extracted Excel/WC.xlsx
+++ b/Extracted Excel/WC.xlsx
@@ -3,37 +3,184 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="23040" windowHeight="8580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
@@ -42,12 +189,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -55,17 +382,306 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -182,7 +798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -215,26 +831,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -267,23 +866,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,12 +1007,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -440,22 +1016,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col width="19.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="32.08984375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="27.08984375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.26953125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="43.81640625" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="12.90625" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="18.7265625" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="16" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="19.3611111111111" customWidth="1" min="2" max="2"/>
+    <col width="32.0925925925926" customWidth="1" min="3" max="3"/>
+    <col width="27.0925925925926" customWidth="1" min="4" max="4"/>
+    <col width="11.2685185185185" customWidth="1" min="5" max="5"/>
+    <col width="43.8148148148148" customWidth="1" min="6" max="6"/>
+    <col width="12.9074074074074" customWidth="1" min="7" max="7"/>
+    <col width="18.7222222222222" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -513,7 +1089,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26-08-2024 20:57:45</t>
+          <t>03-09-2024 21:57:08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -558,7 +1134,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26-08-2024 20:57:51</t>
+          <t>03-09-2024 21:57:14</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -603,7 +1179,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>26-08-2024 20:57:57</t>
+          <t>03-09-2024 21:57:20</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -648,7 +1224,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:02</t>
+          <t>03-09-2024 21:57:26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -693,7 +1269,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:08</t>
+          <t>03-09-2024 21:57:31</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -738,7 +1314,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:14</t>
+          <t>03-09-2024 21:57:37</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -783,7 +1359,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:19</t>
+          <t>03-09-2024 21:57:43</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -828,7 +1404,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:25</t>
+          <t>03-09-2024 21:57:49</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -873,7 +1449,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:31</t>
+          <t>03-09-2024 21:57:55</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -918,7 +1494,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:37</t>
+          <t>03-09-2024 21:58:01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -963,7 +1539,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>26-08-2024 20:58:43</t>
+          <t>03-09-2024 21:58:06</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1008,7 +1584,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>26-08-2024 20:59:57</t>
+          <t>03-09-2024 21:59:19</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1053,7 +1629,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:03</t>
+          <t>03-09-2024 21:59:25</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1098,7 +1674,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:09</t>
+          <t>03-09-2024 21:59:31</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1143,7 +1719,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:15</t>
+          <t>03-09-2024 21:59:37</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1188,7 +1764,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:20</t>
+          <t>03-09-2024 21:59:43</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1233,7 +1809,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:26</t>
+          <t>03-09-2024 21:59:49</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1278,7 +1854,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26-08-2024 21:00:32</t>
+          <t>03-09-2024 21:59:55</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1316,28 +1892,9 @@
           <t>None</t>
         </is>
       </c>
-    </row>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36">
-      <c r="F36" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="1"/>
 </worksheet>
 </file>
</xml_diff>